<commit_message>
Major commit from dev branch
</commit_message>
<xml_diff>
--- a/712dc7592fd9f87b4446d410d04846dae744c676/file/REDF_technical_skills.xlsx
+++ b/712dc7592fd9f87b4446d410d04846dae744c676/file/REDF_technical_skills.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameseddy/PycharmProjects/redf_curriculum_development/redf/docs/file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7D7006-2F91-C040-AC95-20138ED7C6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F48F374-492A-EF44-9983-E30F2DE5F79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36960" yWindow="8740" windowWidth="41980" windowHeight="19780" activeTab="4" xr2:uid="{68765283-6C5F-AA4B-B696-6C20DA08A4EB}"/>
+    <workbookView xWindow="42560" yWindow="7480" windowWidth="41980" windowHeight="19780" activeTab="2" xr2:uid="{68765283-6C5F-AA4B-B696-6C20DA08A4EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Topics (2)" sheetId="8" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="299">
   <si>
     <t>Computer and Device Basics</t>
   </si>
@@ -952,6 +952,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Participants should work toward completion of the following before the next lesson:</t>
   </si>
 </sst>
 </file>
@@ -7535,14 +7538,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{141C6379-715D-4E40-B3EE-EF5053F5DE2A}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="54.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.1640625" customWidth="1"/>
+    <col min="3" max="3" width="53.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -7552,6 +7556,10 @@
       <c r="B1" s="30">
         <v>6.805555555555555E-2</v>
       </c>
+      <c r="C1" t="str">
+        <f>"- "&amp;A1&amp;" *("&amp;TEXT(B1,"H:MM"&amp;")\*")</f>
+        <v>- Networking Foundations: Networking Basics *(1:38)*</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -7560,6 +7568,10 @@
       <c r="B2" s="30">
         <v>8.1944444444444445E-2</v>
       </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C10" si="0">"- "&amp;A2&amp;" *("&amp;TEXT(B2,"H:MM"&amp;")\*")</f>
+        <v>- Computer Components and Peripherals for IT Technicians *(1:58)*</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -7568,6 +7580,10 @@
       <c r="B3" s="30">
         <v>5.9027777777777783E-2</v>
       </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>- Learning Cloud Computing: Core Concepts *(1:25)*</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -7576,6 +7592,10 @@
       <c r="B4" s="30">
         <v>9.0972222222222218E-2</v>
       </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>- Learning Virtualization *(2:11)*</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -7584,6 +7604,10 @@
       <c r="B5" s="30">
         <v>7.2916666666666671E-2</v>
       </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>- Troubleshooting Common PC Issues for Users *(1:45)*</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -7592,6 +7616,10 @@
       <c r="B6" s="30">
         <v>0.12291666666666667</v>
       </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>- CompTIA A+ Core 2 (220-1102) Cert Prep: 3 Operating Systems *(2:57)*</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -7600,6 +7628,10 @@
       <c r="B7" s="30">
         <v>0.29305555555555557</v>
       </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>- LinkedIn Learning/Cert Prep: LPI Linux Essentials (010-160) *(7:02)*</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -7608,6 +7640,10 @@
       <c r="B8" s="30">
         <v>6.5277777777777782E-2</v>
       </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>- LinkedIn Learning/IT Security Foundations: Core Concepts *(1:34)*</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -7616,6 +7652,10 @@
       <c r="B9" s="30">
         <v>8.5416666666666655E-2</v>
       </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>- LinkedIn Learning/IT Help Desk for Beginners *(2:03)*</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -7624,10 +7664,19 @@
       <c r="B10" s="30">
         <v>6.6666666666666666E-2</v>
       </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>- CompTIA A+ Core 1 (220-1101) Cert Prep: 8 Portable Computing *(1:36)*</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" s="29" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -10513,7 +10562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87CEB49F-D3C4-2549-8EAE-31C830ABE1F6}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>